<commit_message>
fixed graphs and conclusions
</commit_message>
<xml_diff>
--- a/PROJ2/covid19_knn_regressor_rank.xlsx
+++ b/PROJ2/covid19_knn_regressor_rank.xlsx
@@ -28,34 +28,34 @@
     <t>MAE</t>
   </si>
   <si>
-    <t>(7, 'distance', 'manhattan', 'kd_tree', 10)</t>
-  </si>
-  <si>
-    <t>(7, 'distance', 'manhattan', 'ball_tree', 10)</t>
-  </si>
-  <si>
-    <t>(7, 'distance', 'manhattan', 'kd_tree', 30)</t>
-  </si>
-  <si>
-    <t>(7, 'distance', 'manhattan', 'kd_tree', 70)</t>
-  </si>
-  <si>
-    <t>(7, 'distance', 'manhattan', 'kd_tree', 150)</t>
-  </si>
-  <si>
-    <t>(3, 'distance', 'manhattan', 'kd_tree', 300)</t>
-  </si>
-  <si>
-    <t>(3, 'distance', 'manhattan', 'ball_tree', 150)</t>
-  </si>
-  <si>
-    <t>(3, 'distance', 'manhattan', 'ball_tree', 300)</t>
-  </si>
-  <si>
-    <t>(3, 'distance', 'manhattan', 'kd_tree', 70)</t>
-  </si>
-  <si>
-    <t>(3, 'distance', 'manhattan', 'ball_tree', 70)</t>
+    <t>(3, 'distance', 'chebyshev', 'brute', 70)</t>
+  </si>
+  <si>
+    <t>(3, 'distance', 'chebyshev', 'brute', 150)</t>
+  </si>
+  <si>
+    <t>(3, 'distance', 'chebyshev', 'brute', 30)</t>
+  </si>
+  <si>
+    <t>(3, 'distance', 'chebyshev', 'brute', 300)</t>
+  </si>
+  <si>
+    <t>(3, 'distance', 'chebyshev', 'brute', 10)</t>
+  </si>
+  <si>
+    <t>(3, 'distance', 'manhattan', 'kd_tree', 10)</t>
+  </si>
+  <si>
+    <t>(3, 'distance', 'manhattan', 'brute', 10)</t>
+  </si>
+  <si>
+    <t>(3, 'distance', 'manhattan', 'kd_tree', 30)</t>
+  </si>
+  <si>
+    <t>(3, 'distance', 'manhattan', 'ball_tree', 30)</t>
+  </si>
+  <si>
+    <t>(3, 'distance', 'manhattan', 'ball_tree', 10)</t>
   </si>
 </sst>
 </file>
@@ -441,13 +441,13 @@
         <v>4</v>
       </c>
       <c r="C2">
-        <v>0.9998017126134032</v>
+        <v>0.9996211712091984</v>
       </c>
       <c r="D2">
-        <v>17624.54871794872</v>
+        <v>31001.32435897436</v>
       </c>
       <c r="E2">
-        <v>17.45641025641025</v>
+        <v>25.11153846153846</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -458,13 +458,13 @@
         <v>5</v>
       </c>
       <c r="C3">
-        <v>0.9998017126134032</v>
+        <v>0.9996211712091984</v>
       </c>
       <c r="D3">
-        <v>17624.54871794872</v>
+        <v>31001.32435897436</v>
       </c>
       <c r="E3">
-        <v>17.45641025641025</v>
+        <v>25.11153846153846</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -475,13 +475,13 @@
         <v>6</v>
       </c>
       <c r="C4">
-        <v>0.9998017126134032</v>
+        <v>0.9996211712091984</v>
       </c>
       <c r="D4">
-        <v>17624.54871794872</v>
+        <v>31001.32435897436</v>
       </c>
       <c r="E4">
-        <v>17.45641025641025</v>
+        <v>25.11153846153846</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -492,13 +492,13 @@
         <v>7</v>
       </c>
       <c r="C5">
-        <v>0.9998017126134032</v>
+        <v>0.9996211712091984</v>
       </c>
       <c r="D5">
-        <v>17624.54871794872</v>
+        <v>31001.32435897436</v>
       </c>
       <c r="E5">
-        <v>17.45641025641025</v>
+        <v>25.11153846153846</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -509,13 +509,13 @@
         <v>8</v>
       </c>
       <c r="C6">
-        <v>0.9998017126134032</v>
+        <v>0.9996211712091984</v>
       </c>
       <c r="D6">
-        <v>17624.54871794872</v>
+        <v>31001.32435897436</v>
       </c>
       <c r="E6">
-        <v>17.45641025641025</v>
+        <v>25.11153846153846</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -526,13 +526,13 @@
         <v>9</v>
       </c>
       <c r="C7">
-        <v>0.9997815687743761</v>
+        <v>0.9995973586037076</v>
       </c>
       <c r="D7">
-        <v>12832.65897435897</v>
+        <v>32408.03076923077</v>
       </c>
       <c r="E7">
-        <v>17.61794871794872</v>
+        <v>21.28974358974359</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -543,13 +543,13 @@
         <v>10</v>
       </c>
       <c r="C8">
-        <v>0.9997815687743761</v>
+        <v>0.9995973586037076</v>
       </c>
       <c r="D8">
-        <v>12832.65897435897</v>
+        <v>32408.03076923077</v>
       </c>
       <c r="E8">
-        <v>17.61794871794872</v>
+        <v>21.28974358974359</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -560,13 +560,13 @@
         <v>11</v>
       </c>
       <c r="C9">
-        <v>0.9997815687743761</v>
+        <v>0.9995973586037076</v>
       </c>
       <c r="D9">
-        <v>12832.65897435897</v>
+        <v>32408.03076923077</v>
       </c>
       <c r="E9">
-        <v>17.61794871794872</v>
+        <v>21.28974358974359</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -577,13 +577,13 @@
         <v>12</v>
       </c>
       <c r="C10">
-        <v>0.9997815681005794</v>
+        <v>0.9995973586037076</v>
       </c>
       <c r="D10">
-        <v>12832.65897435897</v>
+        <v>32408.03076923077</v>
       </c>
       <c r="E10">
-        <v>17.61794871794872</v>
+        <v>21.28974358974359</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -594,13 +594,13 @@
         <v>13</v>
       </c>
       <c r="C11">
-        <v>0.9997815681005794</v>
+        <v>0.9995973586037076</v>
       </c>
       <c r="D11">
-        <v>12832.65897435897</v>
+        <v>32408.03076923077</v>
       </c>
       <c r="E11">
-        <v>17.61794871794872</v>
+        <v>21.28974358974359</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tweaked abstract and intro
</commit_message>
<xml_diff>
--- a/PROJ2/covid19_knn_regressor_rank.xlsx
+++ b/PROJ2/covid19_knn_regressor_rank.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -387,11 +387,6 @@
           <t>MAE</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Time</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -399,20 +394,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>('poly', 1, 10, 'auto')</t>
+          <t>(7, 'distance', 'manhattan', 'kd_tree', 10)</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.8052912305095016</v>
+        <v>0.9999095677851279</v>
       </c>
       <c r="D2" t="n">
-        <v>42958976.67307692</v>
+        <v>6827.301282051281</v>
       </c>
       <c r="E2" t="n">
-        <v>937.9935897435897</v>
-      </c>
-      <c r="F2" t="n">
-        <v>210.0792</v>
+        <v>11.90641025641026</v>
       </c>
     </row>
     <row r="3">
@@ -421,20 +413,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>('poly', 1, 10, 'scale')</t>
+          <t>(7, 'distance', 'manhattan', 'ball_tree', 30)</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.8052912305095016</v>
+        <v>0.9999095677851279</v>
       </c>
       <c r="D3" t="n">
-        <v>42958976.67307692</v>
+        <v>6827.301282051281</v>
       </c>
       <c r="E3" t="n">
-        <v>937.9935897435897</v>
-      </c>
-      <c r="F3" t="n">
-        <v>219.1347</v>
+        <v>11.90641025641026</v>
       </c>
     </row>
     <row r="4">
@@ -443,20 +432,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>('poly', 0.2, 10, 'scale')</t>
+          <t>(7, 'distance', 'manhattan', 'ball_tree', 10)</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.8052550238227575</v>
+        <v>0.9999095677851279</v>
       </c>
       <c r="D4" t="n">
-        <v>42959827.17179487</v>
+        <v>6827.301282051281</v>
       </c>
       <c r="E4" t="n">
-        <v>937.9871794871796</v>
-      </c>
-      <c r="F4" t="n">
-        <v>159.1613</v>
+        <v>11.90641025641026</v>
       </c>
     </row>
     <row r="5">
@@ -465,20 +451,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>('poly', 0.2, 10, 'auto')</t>
+          <t>(7, 'distance', 'manhattan', 'kd_tree', 150)</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.8052550238227575</v>
+        <v>0.9999095677851279</v>
       </c>
       <c r="D5" t="n">
-        <v>42959827.17179487</v>
+        <v>6827.301282051281</v>
       </c>
       <c r="E5" t="n">
-        <v>937.9871794871796</v>
-      </c>
-      <c r="F5" t="n">
-        <v>163.5467</v>
+        <v>11.90641025641026</v>
       </c>
     </row>
     <row r="6">
@@ -487,152 +470,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>('poly', 0.1, 10, 'scale')</t>
+          <t>(7, 'distance', 'manhattan', 'kd_tree', 30)</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.805253914689732</v>
+        <v>0.9999095677851279</v>
       </c>
       <c r="D6" t="n">
-        <v>42959790.01666667</v>
+        <v>6827.301282051281</v>
       </c>
       <c r="E6" t="n">
-        <v>937.9807692307692</v>
-      </c>
-      <c r="F6" t="n">
-        <v>178.7866</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>('poly', 0.1, 10, 'auto')</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>0.805253914689732</v>
-      </c>
-      <c r="D7" t="n">
-        <v>42959790.01666667</v>
-      </c>
-      <c r="E7" t="n">
-        <v>937.9807692307692</v>
-      </c>
-      <c r="F7" t="n">
-        <v>180.5983</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>('poly', 1, 1, 'auto')</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
-        <v>0.6401004985384136</v>
-      </c>
-      <c r="D8" t="n">
-        <v>60958623.00256411</v>
-      </c>
-      <c r="E8" t="n">
-        <v>1116.597435897436</v>
-      </c>
-      <c r="F8" t="n">
-        <v>67.3304</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>('poly', 1, 1, 'scale')</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
-        <v>0.6401004985384136</v>
-      </c>
-      <c r="D9" t="n">
-        <v>60958623.00256411</v>
-      </c>
-      <c r="E9" t="n">
-        <v>1116.597435897436</v>
-      </c>
-      <c r="F9" t="n">
-        <v>67.71080000000001</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>('poly', 0.2, 1, 'auto')</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
-        <v>0.6400445166301774</v>
-      </c>
-      <c r="D10" t="n">
-        <v>60959141.63717949</v>
-      </c>
-      <c r="E10" t="n">
-        <v>1116.59358974359</v>
-      </c>
-      <c r="F10" t="n">
-        <v>91.8192</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>('poly', 0.1, 1, 'auto')</t>
-        </is>
-      </c>
-      <c r="C11" t="n">
-        <v>0.6400441420509662</v>
-      </c>
-      <c r="D11" t="n">
-        <v>60958983.59102565</v>
-      </c>
-      <c r="E11" t="n">
-        <v>1116.585897435898</v>
-      </c>
-      <c r="F11" t="n">
-        <v>62.5515</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>('poly', 0.1, 1, 'scale')</t>
-        </is>
-      </c>
-      <c r="C12" t="n">
-        <v>0.6400441420509662</v>
-      </c>
-      <c r="D12" t="n">
-        <v>60958983.59102565</v>
-      </c>
-      <c r="E12" t="n">
-        <v>1116.585897435898</v>
-      </c>
-      <c r="F12" t="n">
-        <v>62.6059</v>
+        <v>11.90641025641026</v>
       </c>
     </row>
   </sheetData>

</xml_diff>